<commit_message>
week 10 homework complete
</commit_message>
<xml_diff>
--- a/week10/EvenStarFarmRevisited.xlsx
+++ b/week10/EvenStarFarmRevisited.xlsx
@@ -1,15 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="0" windowWidth="18200" windowHeight="15120" tabRatio="500"/>
+    <workbookView xWindow="26440" yWindow="1260" windowWidth="23720" windowHeight="26760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$26:$D$34</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$26:$D$33</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$34:$D$34</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$40:$B$51</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$55</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$B$56</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$B$57</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">6</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$A$37</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">binary</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$D$40:$D$51</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$D$55</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!$D$56</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Sheet1!$D$57</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+  </definedNames>
+  <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>EVEN' STAR ORGANIC PRODUCE</t>
   </si>
@@ -145,6 +191,18 @@
   </si>
   <si>
     <t>CSA limit</t>
+  </si>
+  <si>
+    <t>Participate?</t>
+  </si>
+  <si>
+    <t>Cases to restaurants</t>
+  </si>
+  <si>
+    <t>Cases to Farmer's Mk</t>
+  </si>
+  <si>
+    <t>New Mkt Price</t>
   </si>
 </sst>
 </file>
@@ -154,7 +212,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,6 +224,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -436,10 +510,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -522,8 +612,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -853,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -868,7 +978,7 @@
     <col min="5" max="5" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -877,14 +987,14 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -893,14 +1003,14 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="16" thickBot="1">
+    <row r="4" spans="1:8" ht="16" thickBot="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16" thickBot="1">
+    <row r="5" spans="1:8" ht="31" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -916,8 +1026,11 @@
       <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -931,10 +1044,17 @@
         <v>36</v>
       </c>
       <c r="E6" s="10">
+        <v>47.8125</v>
+      </c>
+      <c r="F6" s="28">
+        <f>E6*1.25</f>
+        <v>59.765625</v>
+      </c>
+      <c r="H6" s="10">
         <v>38.25</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -948,10 +1068,17 @@
         <v>36</v>
       </c>
       <c r="E7" s="10">
+        <v>42.5</v>
+      </c>
+      <c r="F7" s="28">
+        <f t="shared" ref="F7:F13" si="0">E7*1.25</f>
+        <v>53.125</v>
+      </c>
+      <c r="H7" s="10">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -965,10 +1092,17 @@
         <v>20</v>
       </c>
       <c r="E8" s="10">
+        <v>25.3125</v>
+      </c>
+      <c r="F8" s="28">
+        <f t="shared" si="0"/>
+        <v>31.640625</v>
+      </c>
+      <c r="H8" s="10">
         <v>20.25</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:8">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -982,10 +1116,17 @@
         <v>36</v>
       </c>
       <c r="E9" s="10">
+        <v>42.5</v>
+      </c>
+      <c r="F9" s="28">
+        <f t="shared" si="0"/>
+        <v>53.125</v>
+      </c>
+      <c r="H9" s="10">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:8">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -999,10 +1140,17 @@
         <v>24</v>
       </c>
       <c r="E10" s="10">
+        <v>26.5625</v>
+      </c>
+      <c r="F10" s="28">
+        <f t="shared" si="0"/>
+        <v>33.203125</v>
+      </c>
+      <c r="H10" s="10">
         <v>21.25</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1016,10 +1164,17 @@
         <v>24</v>
       </c>
       <c r="E11" s="10">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="28">
+        <f t="shared" si="0"/>
+        <v>39.375</v>
+      </c>
+      <c r="H11" s="10">
         <v>25.2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:8">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -1033,10 +1188,17 @@
         <v>36</v>
       </c>
       <c r="E12" s="10">
+        <v>45</v>
+      </c>
+      <c r="F12" s="28">
+        <f t="shared" si="0"/>
+        <v>56.25</v>
+      </c>
+      <c r="H12" s="10">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1">
+    <row r="13" spans="1:8" ht="16" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
@@ -1050,24 +1212,31 @@
         <v>36</v>
       </c>
       <c r="E13" s="14">
+        <v>45</v>
+      </c>
+      <c r="F13" s="28">
+        <f t="shared" si="0"/>
+        <v>56.25</v>
+      </c>
+      <c r="H13" s="14">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:8">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1176,13 +1345,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="20">
-        <v>406</v>
+        <v>46</v>
       </c>
       <c r="C26" s="21">
         <v>0</v>
       </c>
       <c r="D26" s="22">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -1209,10 +1378,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="19">
+        <v>167</v>
+      </c>
+      <c r="D28" s="24">
         <v>0</v>
-      </c>
-      <c r="D28" s="24">
-        <v>167</v>
       </c>
       <c r="E28" s="2"/>
     </row>
@@ -1254,10 +1423,10 @@
         <v>0</v>
       </c>
       <c r="C31" s="19">
+        <v>251</v>
+      </c>
+      <c r="D31" s="24">
         <v>0</v>
-      </c>
-      <c r="D31" s="24">
-        <v>251</v>
       </c>
       <c r="E31" s="2"/>
     </row>
@@ -1266,13 +1435,13 @@
         <v>13</v>
       </c>
       <c r="B32" s="23">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="C32" s="19">
         <v>0</v>
       </c>
       <c r="D32" s="24">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="E32" s="2"/>
     </row>
@@ -1292,10 +1461,18 @@
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2.5274725274725275E-2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.64505494505494509</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.32967032967032966</v>
+      </c>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5">
@@ -1316,8 +1493,8 @@
     </row>
     <row r="37" spans="1:5" ht="16" thickBot="1">
       <c r="A37" s="15">
-        <f>SUMPRODUCT(B26:D33,C6:E13) - B19*(SUM(B26:B33)/119) - B20 - C19*(SUMPRODUCT(C26:C33,D6:D13)/400) - C20 - D20</f>
-        <v>49956.391768067224</v>
+        <f>SUMPRODUCT(B26:D33,C6:E13) - B19*(SUM(B26:B33)/119) - B34*B20 - C19*(SUMPRODUCT(C26:C33,D6:D13)/400) - C34*C20 - D34*D20</f>
+        <v>60224.772631932778</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1351,7 +1528,7 @@
         <v>30</v>
       </c>
       <c r="B40" s="16">
-        <f>SUM(B26:D26)</f>
+        <f t="shared" ref="B40:B47" si="1">SUM(B26:D26)</f>
         <v>406</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -1367,7 +1544,7 @@
         <v>32</v>
       </c>
       <c r="B41" s="16">
-        <f>SUM(B27:D27)</f>
+        <f t="shared" si="1"/>
         <v>608</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1383,7 +1560,7 @@
         <v>33</v>
       </c>
       <c r="B42" s="16">
-        <f>SUM(B28:D28)</f>
+        <f t="shared" si="1"/>
         <v>167</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -1399,7 +1576,7 @@
         <v>34</v>
       </c>
       <c r="B43" s="16">
-        <f>SUM(B29:D29)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1415,7 +1592,7 @@
         <v>35</v>
       </c>
       <c r="B44" s="16">
-        <f>SUM(B30:D30)</f>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -1431,7 +1608,7 @@
         <v>36</v>
       </c>
       <c r="B45" s="16">
-        <f>SUM(B31:D31)</f>
+        <f t="shared" si="1"/>
         <v>251</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -1447,7 +1624,7 @@
         <v>37</v>
       </c>
       <c r="B46" s="16">
-        <f>SUM(B32:D32)</f>
+        <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -1463,7 +1640,7 @@
         <v>38</v>
       </c>
       <c r="B47" s="16">
-        <f>SUM(B33:D33)</f>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -1503,7 +1680,7 @@
       </c>
       <c r="B50" s="16">
         <f>SUM(B26:B33)/119</f>
-        <v>3.8991596638655461</v>
+        <v>0.38655462184873951</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>31</v>
@@ -1519,7 +1696,7 @@
       </c>
       <c r="B51" s="16">
         <f>SUMPRODUCT(C26:C33,D6:D13)/400</f>
-        <v>65.88</v>
+        <v>89.29</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>31</v>
@@ -1529,8 +1706,63 @@
       </c>
       <c r="E51" s="2"/>
     </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55">
+        <f>SUM(B26:B33)</f>
+        <v>46</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55">
+        <f>B34*1820</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56">
+        <f>SUM(C26:C33)</f>
+        <v>1174</v>
+      </c>
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56">
+        <f>C34*1820</f>
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57">
+        <f>SUM(D26:D33)</f>
+        <v>600</v>
+      </c>
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57">
+        <f>D34*1820</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" s="28">
+        <f>A37-49956.39</f>
+        <v>10268.382631932778</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>